<commit_message>
moved some dates around
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0A3583-4771-D942-8010-5093BF3E78C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A1D611-21D5-F346-9ACC-80D3F37ABDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -192,10 +192,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,9 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +549,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,7 +847,7 @@
         <v>37</v>
       </c>
       <c r="C21" s="1">
-        <v>45364</v>
+        <v>45350</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -853,7 +861,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="1">
-        <v>45363</v>
+        <v>45349</v>
       </c>
       <c r="D22" t="s">
         <v>48</v>
@@ -866,8 +874,8 @@
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="1">
-        <v>45365</v>
+      <c r="C23" s="2">
+        <v>45352</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
changed titles of assignment pages, added instructions for short projects
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A1D611-21D5-F346-9ACC-80D3F37ABDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B929CAF5-7F58-4248-A77A-568C3DD71E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>assessment</t>
   </si>
@@ -183,6 +183,39 @@
   </si>
   <si>
     <t>7pm</t>
+  </si>
+  <si>
+    <t>Short Programming Project 1</t>
+  </si>
+  <si>
+    <t>Short Programming Project 2</t>
+  </si>
+  <si>
+    <t>Short Programming Project 3</t>
+  </si>
+  <si>
+    <t>Short Programming Project 4</t>
+  </si>
+  <si>
+    <t>Short Programming Project 5</t>
+  </si>
+  <si>
+    <t>Short Programming Project 6</t>
+  </si>
+  <si>
+    <t>Short Programming Project 7</t>
+  </si>
+  <si>
+    <t>Short Programming Project 8</t>
+  </si>
+  <si>
+    <t>Short Programming Project 9</t>
+  </si>
+  <si>
+    <t>Short Programming Project 10</t>
+  </si>
+  <si>
+    <t>Short Programming Project 11</t>
   </si>
 </sst>
 </file>
@@ -546,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,13 +667,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>45315</v>
+        <v>45314</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +681,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>45314</v>
@@ -662,13 +695,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1">
-        <v>45316</v>
+        <v>45315</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -676,13 +709,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>45322</v>
+        <v>45316</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -704,10 +737,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1">
-        <v>45323</v>
+        <v>45321</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
@@ -718,10 +751,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1">
-        <v>45329</v>
+        <v>45322</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -732,10 +765,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>45328</v>
+        <v>45323</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -746,10 +779,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>45330</v>
+        <v>45328</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
@@ -760,13 +793,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1">
-        <v>45336</v>
+        <v>45328</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -774,13 +807,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1">
-        <v>45338</v>
+        <v>45329</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -788,10 +821,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
-        <v>45341</v>
+        <v>45330</v>
       </c>
       <c r="D17" t="s">
         <v>48</v>
@@ -802,10 +835,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
-        <v>45343</v>
+        <v>45336</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -816,10 +849,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1">
-        <v>45342</v>
+        <v>45338</v>
       </c>
       <c r="D19" t="s">
         <v>48</v>
@@ -830,10 +863,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1">
-        <v>45344</v>
+        <v>45338</v>
       </c>
       <c r="D20" t="s">
         <v>48</v>
@@ -844,13 +877,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1">
-        <v>45350</v>
+        <v>45341</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -858,10 +891,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>45349</v>
+        <v>45342</v>
       </c>
       <c r="D22" t="s">
         <v>48</v>
@@ -872,10 +905,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="2">
-        <v>45352</v>
+        <v>53</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45342</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>
@@ -886,10 +919,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1">
-        <v>45371</v>
+        <v>45343</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -900,10 +933,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1">
-        <v>45370</v>
+        <v>45344</v>
       </c>
       <c r="D25" t="s">
         <v>48</v>
@@ -914,10 +947,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1">
-        <v>45372</v>
+        <v>45349</v>
       </c>
       <c r="D26" t="s">
         <v>48</v>
@@ -928,13 +961,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1">
-        <v>45378</v>
+        <v>45349</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,13 +975,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1">
-        <v>45379</v>
+        <v>45350</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -956,10 +989,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1">
-        <v>45384</v>
+        <v>20</v>
+      </c>
+      <c r="C29" s="2">
+        <v>45352</v>
       </c>
       <c r="D29" t="s">
         <v>48</v>
@@ -971,13 +1004,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C30" s="1">
-        <v>45385</v>
+        <v>45370</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -985,10 +1018,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1">
-        <v>45386</v>
+        <v>45370</v>
       </c>
       <c r="D31" t="s">
         <v>48</v>
@@ -999,13 +1032,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1">
-        <v>45391</v>
+        <v>45371</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1014,13 +1047,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1">
-        <v>45392</v>
+        <v>45372</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,13 +1061,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1">
-        <v>45393</v>
+        <v>45378</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,10 +1075,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1">
-        <v>45398</v>
+        <v>45379</v>
       </c>
       <c r="D35" t="s">
         <v>48</v>
@@ -1056,13 +1089,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C36" s="1">
-        <v>45399</v>
+        <v>45384</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,10 +1103,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1">
-        <v>45400</v>
+        <v>45384</v>
       </c>
       <c r="D37" t="s">
         <v>48</v>
@@ -1084,10 +1117,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1">
-        <v>45406</v>
+        <v>45385</v>
       </c>
       <c r="D38" t="s">
         <v>46</v>
@@ -1098,10 +1131,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1">
-        <v>45407</v>
+        <v>45386</v>
       </c>
       <c r="D39" t="s">
         <v>48</v>
@@ -1112,10 +1145,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1">
-        <v>45412</v>
+        <v>45391</v>
       </c>
       <c r="D40" t="s">
         <v>48</v>
@@ -1126,13 +1159,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C41" s="1">
-        <v>45413</v>
+        <v>45391</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,13 +1173,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C42" s="1">
-        <v>45413</v>
+        <v>45392</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,20 +1187,177 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="1">
+        <v>45393</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="1">
+        <v>45398</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="1">
+        <v>45398</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="1">
+        <v>45399</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="1">
+        <v>45400</v>
+      </c>
+      <c r="D47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="1">
+        <v>45406</v>
+      </c>
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="1">
+        <v>45407</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="1">
+        <v>45412</v>
+      </c>
+      <c r="D50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="1">
+        <v>45412</v>
+      </c>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" s="1">
+        <v>45413</v>
+      </c>
+      <c r="D52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="1">
+        <v>45413</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C54" s="1">
         <v>45415</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D54" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="1"/>
+      <c r="C55"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D59">
+    <sortCondition ref="C2:C59"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added short projects section
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B929CAF5-7F58-4248-A77A-568C3DD71E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D6516F-645B-E241-B362-C5988DEDF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>in class</t>
   </si>
   <si>
-    <t>ENR2 N120</t>
-  </si>
-  <si>
     <t>7pm</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>Short Programming Project 11</t>
+  </si>
+  <si>
+    <t>TBA</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,7 +631,7 @@
         <v>45303</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,7 +659,7 @@
         <v>45309</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -673,7 +673,7 @@
         <v>45314</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -681,13 +681,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1">
         <v>45314</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
         <v>45316</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -729,7 +729,7 @@
         <v>45321</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -737,13 +737,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1">
         <v>45321</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -771,7 +771,7 @@
         <v>45323</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -785,7 +785,7 @@
         <v>45328</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -793,13 +793,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1">
         <v>45328</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,7 +827,7 @@
         <v>45330</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>45338</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -863,13 +863,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1">
         <v>45338</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
         <v>45341</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -897,7 +897,7 @@
         <v>45342</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -905,13 +905,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1">
         <v>45342</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -939,7 +939,7 @@
         <v>45344</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -953,7 +953,7 @@
         <v>45349</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -961,13 +961,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="1">
         <v>45349</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -995,7 +995,7 @@
         <v>45352</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -1010,7 +1010,7 @@
         <v>45370</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1018,13 +1018,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1">
         <v>45370</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>45372</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
         <v>45379</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1095,7 +1095,7 @@
         <v>45384</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1103,13 +1103,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1">
         <v>45384</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1137,7 +1137,7 @@
         <v>45386</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1151,7 +1151,7 @@
         <v>45391</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1159,13 +1159,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" s="1">
         <v>45391</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1193,7 +1193,7 @@
         <v>45393</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1207,7 +1207,7 @@
         <v>45398</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1215,13 +1215,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1">
         <v>45398</v>
       </c>
       <c r="D45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>45400</v>
       </c>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1277,7 +1277,7 @@
         <v>45407</v>
       </c>
       <c r="D49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1291,7 +1291,7 @@
         <v>45412</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1299,13 +1299,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" s="1">
         <v>45412</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1333,7 +1333,7 @@
         <v>45413</v>
       </c>
       <c r="D53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1347,7 +1347,7 @@
         <v>45415</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
shifted due dates a bit
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5299A8-AF35-D14B-9CCF-36B110156A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C004C37-1E5F-D947-BD6D-50FA23E7CD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,13 +905,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1">
-        <v>45342</v>
+        <v>45343</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -919,13 +919,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
-        <v>45343</v>
+        <v>45349</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -933,10 +933,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1">
-        <v>45344</v>
+        <v>45349</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
@@ -947,13 +947,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -961,27 +961,28 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="1">
-        <v>45349</v>
+        <v>18</v>
+      </c>
+      <c r="C27" s="2">
+        <v>45351</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
       </c>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C28" s="1">
-        <v>45350</v>
+        <v>45356</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -991,13 +992,12 @@
       <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="2">
-        <v>45351</v>
+      <c r="C29" s="1">
+        <v>45358</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1012,6 +1012,7 @@
       <c r="D30" t="s">
         <v>47</v>
       </c>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1040,7 +1041,6 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1355,8 +1355,8 @@
       <c r="C55"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D59">
-    <sortCondition ref="C2:C59"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
+    <sortCondition ref="C2:C57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
skipped over spring break for due dates
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C004C37-1E5F-D947-BD6D-50FA23E7CD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432DE873-A98C-3A4B-8B22-847E1B882CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A54"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,7 +979,7 @@
         <v>53</v>
       </c>
       <c r="C28" s="1">
-        <v>45356</v>
+        <v>45363</v>
       </c>
       <c r="D28" t="s">
         <v>47</v>
@@ -993,7 +993,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="1">
-        <v>45358</v>
+        <v>45365</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
added final exam room information
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432DE873-A98C-3A4B-8B22-847E1B882CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB0C501-C8A4-B04B-AFEA-ADF4FE868929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -215,7 +215,7 @@
     <t>Short Programming Project 11</t>
   </si>
   <si>
-    <t>TBA</t>
+    <t>ENR2 N120</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
re-rendered everything due to the change of room for the final exam
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4123CD-46EC-6344-81C7-FCB14C3E2A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68479E08-7FCB-4148-B805-E0FB4D31B00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33480" yWindow="-200" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
     <t>Short Programming Project 11</t>
   </si>
   <si>
-    <t>ENR2 N120</t>
+    <t>CESL 102 and 103</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed dates from fall 2024
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68479E08-7FCB-4148-B805-E0FB4D31B00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826770C-EDD4-5D4C-84A8-C8A5E5312301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="-36060" yWindow="1060" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
   <si>
     <t>assessment</t>
   </si>
@@ -215,7 +215,130 @@
     <t>Short Programming Project 11</t>
   </si>
   <si>
-    <t>CESL 102 and 103</t>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-08-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-08-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-09-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-10-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-11-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-12-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-12-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-12-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-12-11</t>
   </si>
 </sst>
 </file>
@@ -261,10 +384,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,17 +703,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -599,7 +723,7 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
@@ -613,8 +737,8 @@
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1">
-        <v>45301</v>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -627,8 +751,8 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>45303</v>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -641,8 +765,8 @@
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1">
-        <v>45308</v>
+      <c r="C4" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -655,8 +779,8 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
-        <v>45309</v>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -669,8 +793,8 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
-        <v>45314</v>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D6" t="s">
         <v>47</v>
@@ -683,8 +807,8 @@
       <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="1">
-        <v>45314</v>
+      <c r="C7" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
@@ -697,8 +821,8 @@
       <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1">
-        <v>45315</v>
+      <c r="C8" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -711,8 +835,8 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1">
-        <v>45316</v>
+      <c r="C9" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -725,8 +849,8 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
-        <v>45321</v>
+      <c r="C10" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>47</v>
@@ -739,8 +863,8 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="1">
-        <v>45321</v>
+      <c r="C11" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -753,8 +877,8 @@
       <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1">
-        <v>45322</v>
+      <c r="C12" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -767,8 +891,8 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
-        <v>45323</v>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
@@ -781,8 +905,8 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1">
-        <v>45328</v>
+      <c r="C14" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -795,8 +919,8 @@
       <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="1">
-        <v>45328</v>
+      <c r="C15" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -809,458 +933,458 @@
       <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="1">
-        <v>45329</v>
+      <c r="C16" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="1">
-        <v>45330</v>
+      <c r="C17" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1">
-        <v>45336</v>
+      <c r="C18" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1">
-        <v>45338</v>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1">
-        <v>45338</v>
+      <c r="C20" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="1">
-        <v>45341</v>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="1">
-        <v>45342</v>
+      <c r="C22" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="1">
-        <v>45343</v>
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="1">
-        <v>45349</v>
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="1">
-        <v>45349</v>
+        <v>18</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1">
-        <v>45350</v>
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="2">
-        <v>45351</v>
+        <v>53</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="1">
-        <v>45363</v>
+        <v>37</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="1">
-        <v>45365</v>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="1">
-        <v>45370</v>
+        <v>22</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1">
-        <v>45370</v>
+        <v>14</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="1">
-        <v>45364</v>
+        <v>16</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="1">
-        <v>45372</v>
+        <v>54</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="1">
-        <v>45378</v>
+        <v>38</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="1">
-        <v>45379</v>
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="1">
-        <v>45384</v>
+      <c r="C36" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D36" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="1">
-        <v>45384</v>
+      <c r="C37" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="1">
-        <v>45371</v>
+      <c r="C38" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="1">
-        <v>45386</v>
+      <c r="C39" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="1">
-        <v>45391</v>
+      <c r="C40" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="1">
-        <v>45391</v>
+      <c r="C41" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="1">
-        <v>45385</v>
+      <c r="C42" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="1">
-        <v>45393</v>
+      <c r="C43" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="1">
-        <v>45398</v>
+        <v>23</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="1">
-        <v>45398</v>
+        <v>44</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="1">
-        <v>45392</v>
-      </c>
-      <c r="D46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="1">
-        <v>45400</v>
-      </c>
-      <c r="D47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="1">
-        <v>45406</v>
+      <c r="C48" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D48" t="s">
         <v>46</v>
@@ -1271,10 +1395,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" s="1">
-        <v>45407</v>
+        <v>28</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="D49" t="s">
         <v>47</v>
@@ -1287,8 +1411,8 @@
       <c r="B50" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="1">
-        <v>45412</v>
+      <c r="C50" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D50" t="s">
         <v>47</v>
@@ -1301,8 +1425,8 @@
       <c r="B51" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="1">
-        <v>45412</v>
+      <c r="C51" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -1315,8 +1439,8 @@
       <c r="B52" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="1">
-        <v>45399</v>
+      <c r="C52" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D52" t="s">
         <v>46</v>
@@ -1329,8 +1453,8 @@
       <c r="B53" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="1">
-        <v>45413</v>
+      <c r="C53" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D53" t="s">
         <v>47</v>
@@ -1343,8 +1467,8 @@
       <c r="B54" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="1">
-        <v>45415</v>
+      <c r="C54" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D54" t="s">
         <v>59</v>
@@ -1352,11 +1476,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
-      <c r="C55"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
-    <sortCondition ref="C2:C57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D66">
+    <sortCondition ref="C2:C66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed midterm 1 date
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826770C-EDD4-5D4C-84A8-C8A5E5312301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99393A01-DA02-7A44-8766-62E6048A1EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36060" yWindow="1060" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,11 +384,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,14 +705,13 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +721,7 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
@@ -737,7 +735,7 @@
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>60</v>
       </c>
       <c r="D2" t="s">
@@ -751,7 +749,7 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>61</v>
       </c>
       <c r="D3" t="s">
@@ -765,7 +763,7 @@
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>62</v>
       </c>
       <c r="D4" t="s">
@@ -779,7 +777,7 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>63</v>
       </c>
       <c r="D5" t="s">
@@ -793,7 +791,7 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>64</v>
       </c>
       <c r="D6" t="s">
@@ -807,7 +805,7 @@
       <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>64</v>
       </c>
       <c r="D7" t="s">
@@ -821,7 +819,7 @@
       <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>65</v>
       </c>
       <c r="D8" t="s">
@@ -835,7 +833,7 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>66</v>
       </c>
       <c r="D9" t="s">
@@ -849,7 +847,7 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>67</v>
       </c>
       <c r="D10" t="s">
@@ -863,7 +861,7 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>67</v>
       </c>
       <c r="D11" t="s">
@@ -877,7 +875,7 @@
       <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>68</v>
       </c>
       <c r="D12" t="s">
@@ -891,7 +889,7 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>69</v>
       </c>
       <c r="D13" t="s">
@@ -905,7 +903,7 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>70</v>
       </c>
       <c r="D14" t="s">
@@ -919,7 +917,7 @@
       <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>70</v>
       </c>
       <c r="D15" t="s">
@@ -933,7 +931,7 @@
       <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>71</v>
       </c>
       <c r="D16" t="s">
@@ -947,7 +945,7 @@
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>72</v>
       </c>
       <c r="D17" t="s">
@@ -961,7 +959,7 @@
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>73</v>
       </c>
       <c r="D18" t="s">
@@ -975,7 +973,7 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>74</v>
       </c>
       <c r="D19" t="s">
@@ -989,7 +987,7 @@
       <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>75</v>
       </c>
       <c r="D20" t="s">
@@ -1003,7 +1001,7 @@
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>76</v>
       </c>
       <c r="D21" t="s">
@@ -1017,7 +1015,7 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>77</v>
       </c>
       <c r="D22" t="s">
@@ -1031,7 +1029,7 @@
       <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>77</v>
       </c>
       <c r="D23" t="s">
@@ -1045,7 +1043,7 @@
       <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>78</v>
       </c>
       <c r="D24" t="s">
@@ -1059,7 +1057,7 @@
       <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D25" t="s">
@@ -1073,7 +1071,7 @@
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>80</v>
       </c>
       <c r="D26" t="s">
@@ -1087,7 +1085,7 @@
       <c r="B27" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>80</v>
       </c>
       <c r="D27" t="s">
@@ -1101,7 +1099,7 @@
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>81</v>
       </c>
       <c r="D28" t="s">
@@ -1115,7 +1113,7 @@
       <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>82</v>
       </c>
       <c r="D29" t="s">
@@ -1129,7 +1127,7 @@
       <c r="B30" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>83</v>
       </c>
       <c r="D30" t="s">
@@ -1143,7 +1141,7 @@
       <c r="B31" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>84</v>
       </c>
       <c r="D31" t="s">
@@ -1157,7 +1155,7 @@
       <c r="B32" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>85</v>
       </c>
       <c r="D32" t="s">
@@ -1171,7 +1169,7 @@
       <c r="B33" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>85</v>
       </c>
       <c r="D33" t="s">
@@ -1185,7 +1183,7 @@
       <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" t="s">
         <v>86</v>
       </c>
       <c r="D34" t="s">
@@ -1199,7 +1197,7 @@
       <c r="B35" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" t="s">
         <v>87</v>
       </c>
       <c r="D35" t="s">
@@ -1213,7 +1211,7 @@
       <c r="B36" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" t="s">
         <v>88</v>
       </c>
       <c r="D36" t="s">
@@ -1228,7 +1226,7 @@
       <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" t="s">
         <v>88</v>
       </c>
       <c r="D37" t="s">
@@ -1242,7 +1240,7 @@
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>89</v>
       </c>
       <c r="D38" t="s">
@@ -1256,7 +1254,7 @@
       <c r="B39" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>90</v>
       </c>
       <c r="D39" t="s">
@@ -1271,7 +1269,7 @@
       <c r="B40" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>91</v>
       </c>
       <c r="D40" t="s">
@@ -1285,7 +1283,7 @@
       <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>91</v>
       </c>
       <c r="D41" t="s">
@@ -1299,7 +1297,7 @@
       <c r="B42" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
         <v>92</v>
       </c>
       <c r="D42" t="s">
@@ -1313,7 +1311,7 @@
       <c r="B43" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" t="s">
         <v>93</v>
       </c>
       <c r="D43" t="s">
@@ -1327,7 +1325,7 @@
       <c r="B44" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
         <v>94</v>
       </c>
       <c r="D44" t="s">
@@ -1341,7 +1339,7 @@
       <c r="B45" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" t="s">
         <v>95</v>
       </c>
       <c r="D45" t="s">
@@ -1355,7 +1353,7 @@
       <c r="B46" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" t="s">
         <v>96</v>
       </c>
       <c r="D46" t="s">
@@ -1369,7 +1367,7 @@
       <c r="B47" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" t="s">
         <v>96</v>
       </c>
       <c r="D47" t="s">
@@ -1383,7 +1381,7 @@
       <c r="B48" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" t="s">
         <v>97</v>
       </c>
       <c r="D48" t="s">
@@ -1397,7 +1395,7 @@
       <c r="B49" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" t="s">
         <v>98</v>
       </c>
       <c r="D49" t="s">
@@ -1411,7 +1409,7 @@
       <c r="B50" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" t="s">
         <v>99</v>
       </c>
       <c r="D50" t="s">
@@ -1425,7 +1423,7 @@
       <c r="B51" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" t="s">
         <v>99</v>
       </c>
       <c r="D51" t="s">
@@ -1439,7 +1437,7 @@
       <c r="B52" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" t="s">
         <v>100</v>
       </c>
       <c r="D52" t="s">
@@ -1453,7 +1451,7 @@
       <c r="B53" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" t="s">
         <v>100</v>
       </c>
       <c r="D53" t="s">
@@ -1467,7 +1465,7 @@
       <c r="B54" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" t="s">
         <v>59</v>
       </c>
       <c r="D54" t="s">

</xml_diff>

<commit_message>
updated syllabus and first set of slides
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99393A01-DA02-7A44-8766-62E6048A1EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FBD806-F038-CE4F-9F07-D691917E7E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>assessment</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 2024-12-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2024-12-13</t>
   </si>
 </sst>
 </file>
@@ -704,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1466,7 +1469,7 @@
         <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
addd final exam room information
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FBD806-F038-CE4F-9F07-D691917E7E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2AB3C3-F0D7-EF45-894A-31555EDE0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>Short Programming Project 11</t>
   </si>
   <si>
-    <t>TBA</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2024-08-28</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 2024-12-13</t>
+  </si>
+  <si>
+    <t>6pm S SCI 100</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,7 +739,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -767,7 +767,7 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -781,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -795,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>47</v>
@@ -809,7 +809,7 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
@@ -823,7 +823,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -837,7 +837,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -851,7 +851,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
         <v>47</v>
@@ -865,7 +865,7 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -879,7 +879,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -893,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
@@ -907,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -921,7 +921,7 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -935,7 +935,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
@@ -949,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -963,7 +963,7 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -991,7 +991,7 @@
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
         <v>47</v>
@@ -1005,7 +1005,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
@@ -1019,7 +1019,7 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
@@ -1033,7 +1033,7 @@
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
         <v>47</v>
@@ -1047,7 +1047,7 @@
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -1061,7 +1061,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
@@ -1075,7 +1075,7 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
@@ -1089,7 +1089,7 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
@@ -1103,7 +1103,7 @@
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -1117,7 +1117,7 @@
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
@@ -1131,7 +1131,7 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -1145,7 +1145,7 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
         <v>47</v>
@@ -1159,7 +1159,7 @@
         <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
@@ -1173,7 +1173,7 @@
         <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
         <v>47</v>
@@ -1187,7 +1187,7 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
@@ -1201,7 +1201,7 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
         <v>47</v>
@@ -1215,7 +1215,7 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
         <v>47</v>
@@ -1230,7 +1230,7 @@
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
@@ -1244,7 +1244,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
         <v>46</v>
@@ -1258,7 +1258,7 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -1273,7 +1273,7 @@
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
         <v>47</v>
@@ -1287,7 +1287,7 @@
         <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
         <v>47</v>
@@ -1301,7 +1301,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
         <v>46</v>
@@ -1315,7 +1315,7 @@
         <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
         <v>47</v>
@@ -1329,7 +1329,7 @@
         <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1343,7 +1343,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1357,7 +1357,7 @@
         <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
         <v>47</v>
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D47" t="s">
         <v>47</v>
@@ -1385,7 +1385,7 @@
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
         <v>46</v>
@@ -1399,7 +1399,7 @@
         <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
         <v>47</v>
@@ -1413,7 +1413,7 @@
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D50" t="s">
         <v>47</v>
@@ -1427,7 +1427,7 @@
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -1441,7 +1441,7 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
         <v>46</v>
@@ -1455,7 +1455,7 @@
         <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
         <v>47</v>
@@ -1469,10 +1469,10 @@
         <v>24</v>
       </c>
       <c r="C54" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" t="s">
         <v>101</v>
-      </c>
-      <c r="D54" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>